<commit_message>
test(func): Move to new sample data
</commit_message>
<xml_diff>
--- a/YoFi.Tests.Functional/SampleData/SampleData-2022-Upload-Tx.xlsx
+++ b/YoFi.Tests.Functional/SampleData/SampleData-2022-Upload-Tx.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Transaction" sheetId="1" r:id="R28a98aa8ade24b5e"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Split" sheetId="2" r:id="R9ec4b5eebb43453d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Transaction" sheetId="1" r:id="R2afce6df634c41c4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Split" sheetId="2" r:id="R68299bed4677475e"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -172,7 +172,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="1" t="n">
-        <x:v>44567</x:v>
+        <x:v>44572</x:v>
       </x:c>
       <x:c r="C2" t="s">
         <x:v>15</x:v>
@@ -195,7 +195,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B3" s="1" t="n">
-        <x:v>44574</x:v>
+        <x:v>44584</x:v>
       </x:c>
       <x:c r="C3" t="s">
         <x:v>16</x:v>
@@ -221,7 +221,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B4" s="1" t="n">
-        <x:v>44598</x:v>
+        <x:v>44603</x:v>
       </x:c>
       <x:c r="C4" t="s">
         <x:v>15</x:v>
@@ -244,7 +244,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B5" s="1" t="n">
-        <x:v>44605</x:v>
+        <x:v>44615</x:v>
       </x:c>
       <x:c r="C5" t="s">
         <x:v>16</x:v>
@@ -270,7 +270,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B6" s="1" t="n">
-        <x:v>44626</x:v>
+        <x:v>44631</x:v>
       </x:c>
       <x:c r="C6" t="s">
         <x:v>15</x:v>
@@ -293,7 +293,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B7" s="1" t="n">
-        <x:v>44633</x:v>
+        <x:v>44643</x:v>
       </x:c>
       <x:c r="C7" t="s">
         <x:v>16</x:v>
@@ -319,7 +319,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B8" s="1" t="n">
-        <x:v>44657</x:v>
+        <x:v>44662</x:v>
       </x:c>
       <x:c r="C8" t="s">
         <x:v>15</x:v>
@@ -342,7 +342,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B9" s="1" t="n">
-        <x:v>44664</x:v>
+        <x:v>44674</x:v>
       </x:c>
       <x:c r="C9" t="s">
         <x:v>16</x:v>
@@ -368,7 +368,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B10" s="1" t="n">
-        <x:v>44687</x:v>
+        <x:v>44692</x:v>
       </x:c>
       <x:c r="C10" t="s">
         <x:v>15</x:v>
@@ -391,7 +391,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B11" s="1" t="n">
-        <x:v>44694</x:v>
+        <x:v>44704</x:v>
       </x:c>
       <x:c r="C11" t="s">
         <x:v>16</x:v>
@@ -417,7 +417,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B12" s="1" t="n">
-        <x:v>44718</x:v>
+        <x:v>44723</x:v>
       </x:c>
       <x:c r="C12" t="s">
         <x:v>15</x:v>
@@ -440,16 +440,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B13" s="1" t="n">
-        <x:v>44725</x:v>
+        <x:v>44730</x:v>
       </x:c>
       <x:c r="C13" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D13" s="2" t="n">
-        <x:v>-250</x:v>
+        <x:v>-4000</x:v>
       </x:c>
       <x:c r="E13" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="M13" t="b">
         <x:v>0</x:v>
@@ -458,105 +458,105 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="O13" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="">
       <x:c r="A14" t="n">
-        <x:v>7</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B14" s="1" t="n">
-        <x:v>44748</x:v>
+        <x:v>44735</x:v>
       </x:c>
       <x:c r="C14" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D14" s="2" t="n">
-        <x:v>-250.00</x:v>
+        <x:v>-250</x:v>
+      </x:c>
+      <x:c r="E14" t="s">
+        <x:v>17</x:v>
       </x:c>
       <x:c r="M14" t="b">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="N14" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="O14" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="">
       <x:c r="A15" t="n">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B15" s="1" t="n">
-        <x:v>44755</x:v>
+        <x:v>44753</x:v>
       </x:c>
       <x:c r="C15" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D15" s="2" t="n">
-        <x:v>-250</x:v>
-      </x:c>
-      <x:c r="E15" t="s">
-        <x:v>17</x:v>
+        <x:v>-250.00</x:v>
       </x:c>
       <x:c r="M15" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="N15" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="O15" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="">
       <x:c r="A16" t="n">
-        <x:v>8</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B16" s="1" t="n">
-        <x:v>44779</x:v>
+        <x:v>44765</x:v>
       </x:c>
       <x:c r="C16" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D16" s="2" t="n">
-        <x:v>-250.00</x:v>
+        <x:v>-250</x:v>
+      </x:c>
+      <x:c r="E16" t="s">
+        <x:v>17</x:v>
       </x:c>
       <x:c r="M16" t="b">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="N16" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="O16" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="">
       <x:c r="A17" t="n">
-        <x:v>0</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B17" s="1" t="n">
-        <x:v>44786</x:v>
+        <x:v>44784</x:v>
       </x:c>
       <x:c r="C17" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D17" s="2" t="n">
-        <x:v>-250</x:v>
-      </x:c>
-      <x:c r="E17" t="s">
-        <x:v>17</x:v>
+        <x:v>-250.00</x:v>
       </x:c>
       <x:c r="M17" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="N17" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="O17" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="">
@@ -564,16 +564,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B18" s="1" t="n">
-        <x:v>44794</x:v>
+        <x:v>44796</x:v>
       </x:c>
       <x:c r="C18" t="s">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D18" s="2" t="n">
-        <x:v>-4000</x:v>
+        <x:v>-250</x:v>
       </x:c>
       <x:c r="E18" t="s">
-        <x:v>19</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="M18" t="b">
         <x:v>0</x:v>
@@ -582,7 +582,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="O18" t="s">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="">
@@ -590,7 +590,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B19" s="1" t="n">
-        <x:v>44810</x:v>
+        <x:v>44815</x:v>
       </x:c>
       <x:c r="C19" t="s">
         <x:v>15</x:v>
@@ -613,7 +613,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B20" s="1" t="n">
-        <x:v>44817</x:v>
+        <x:v>44827</x:v>
       </x:c>
       <x:c r="C20" t="s">
         <x:v>16</x:v>
@@ -639,7 +639,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B21" s="1" t="n">
-        <x:v>44840</x:v>
+        <x:v>44845</x:v>
       </x:c>
       <x:c r="C21" t="s">
         <x:v>15</x:v>
@@ -662,7 +662,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B22" s="1" t="n">
-        <x:v>44847</x:v>
+        <x:v>44857</x:v>
       </x:c>
       <x:c r="C22" t="s">
         <x:v>16</x:v>
@@ -688,7 +688,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B23" s="1" t="n">
-        <x:v>44871</x:v>
+        <x:v>44876</x:v>
       </x:c>
       <x:c r="C23" t="s">
         <x:v>15</x:v>
@@ -711,7 +711,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B24" s="1" t="n">
-        <x:v>44878</x:v>
+        <x:v>44888</x:v>
       </x:c>
       <x:c r="C24" t="s">
         <x:v>16</x:v>
@@ -737,7 +737,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B25" s="1" t="n">
-        <x:v>44901</x:v>
+        <x:v>44906</x:v>
       </x:c>
       <x:c r="C25" t="s">
         <x:v>15</x:v>
@@ -760,7 +760,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B26" s="1" t="n">
-        <x:v>44908</x:v>
+        <x:v>44918</x:v>
       </x:c>
       <x:c r="C26" t="s">
         <x:v>16</x:v>

</xml_diff>